<commit_message>
Have two sites to download
</commit_message>
<xml_diff>
--- a/config/example.xlsx
+++ b/config/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">Organization</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">www.fso-bremen.de</t>
-  </si>
-  <si>
-    <t xml:space="preserve">done</t>
   </si>
   <si>
     <t xml:space="preserve">fso-bremen.de</t>
@@ -162,7 +159,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -197,16 +194,13 @@
       <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement additional folder column for naming files
</commit_message>
<xml_diff>
--- a/config/example.xlsx
+++ b/config/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">Organization</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Url</t>
   </si>
   <si>
+    <t xml:space="preserve">Folder</t>
+  </si>
+  <si>
     <t xml:space="preserve">SizeWarc</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">www.fso-bremen.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forschungsstelle Osteuropa</t>
   </si>
   <si>
     <t xml:space="preserve">fso-bremen.de</t>
@@ -156,15 +162,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -186,21 +194,27 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add timedelta of subprocess start and end to SQLite
</commit_message>
<xml_diff>
--- a/config/example.xlsx
+++ b/config/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t xml:space="preserve">Organization</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">SizeLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DownloadDelta</t>
   </si>
   <si>
     <t xml:space="preserve">Last</t>
@@ -162,17 +165,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -197,24 +202,27 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>